<commit_message>
fix bug with dist/linear distribution (needed integer arrays)
</commit_message>
<xml_diff>
--- a/AssessmentSchedule_2425.xlsx
+++ b/AssessmentSchedule_2425.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/northce_cardiff_ac_uk/Documents/Documents/Cardiff/DUGS/Assessments/Schedule Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2180" documentId="8_{F6E35C1D-54A9-4F6E-BB8B-E8E1539C4BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{239008D7-3BD6-46EE-A49D-E5A4BBC966F0}"/>
+  <xr:revisionPtr revIDLastSave="2184" documentId="8_{F6E35C1D-54A9-4F6E-BB8B-E8E1539C4BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66721BFC-2AF1-4B04-96CA-78D631A9CA39}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="2" xr2:uid="{A20BCC1C-F123-4C76-9181-B345A7D760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="11" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -8634,7 +8634,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3F344565-A902-475D-ACD8-7DA2FB255CBD}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B70" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="34">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -9544,8 +9544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66039B40-29AD-4D93-B125-EAF72A7B3996}">
   <dimension ref="A1:AJ144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
@@ -27382,8 +27382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D548CE7-BEAC-43FA-847F-FDE82E3A5926}">
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -31936,8 +31936,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H2:N98">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="O">
+      <formula>NOT(ISERROR(SEARCH("O",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G2:G98">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="10"/>
         <cfvo type="percentile" val="50"/>
@@ -31946,14 +31954,6 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:N98">
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="O">
-      <formula>NOT(ISERROR(SEARCH("O",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="C">
-      <formula>NOT(ISERROR(SEARCH("C",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>